<commit_message>
Added CSV's and timemaps to the scr_data and timemaps folders
</commit_message>
<xml_diff>
--- a/src_data/famu.xlsx
+++ b/src_data/famu.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18656\Desktop\datacollection\src_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE59DAD0-3898-43CB-8EE5-1343336CE66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
   <si>
     <t>Department</t>
   </si>
@@ -274,24 +283,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -299,7 +312,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -309,38 +322,41 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -530,20 +546,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -559,7 +580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -567,7 +588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -575,7 +596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -583,7 +604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -591,15 +612,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -607,31 +626,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -639,7 +652,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -647,7 +660,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -655,7 +668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -663,7 +676,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -671,7 +684,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -679,7 +692,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
@@ -687,7 +700,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -695,7 +708,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -703,7 +716,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -711,7 +724,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
@@ -719,7 +732,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -727,7 +740,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
@@ -735,7 +748,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>45</v>
       </c>
@@ -743,7 +756,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>47</v>
       </c>
@@ -751,7 +764,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
@@ -759,7 +772,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -767,7 +780,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>53</v>
       </c>
@@ -775,7 +788,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>55</v>
       </c>
@@ -783,7 +796,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>57</v>
       </c>
@@ -791,7 +804,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>59</v>
       </c>
@@ -799,7 +812,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>61</v>
       </c>
@@ -807,7 +820,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
@@ -815,7 +828,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
@@ -823,7 +836,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -831,7 +844,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>69</v>
       </c>
@@ -839,7 +852,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>71</v>
       </c>
@@ -847,7 +860,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>73</v>
       </c>
@@ -855,7 +868,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>75</v>
       </c>
@@ -863,7 +876,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>77</v>
       </c>
@@ -871,7 +884,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>78</v>
       </c>
@@ -879,7 +892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>79</v>
       </c>
@@ -887,7 +900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>80</v>
       </c>
@@ -895,7 +908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>81</v>
       </c>
@@ -903,7 +916,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>82</v>
       </c>
@@ -911,7 +924,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>84</v>
       </c>
@@ -921,44 +934,44 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B8"/>
-    <hyperlink r:id="rId7" ref="B12"/>
-    <hyperlink r:id="rId8" ref="B13"/>
-    <hyperlink r:id="rId9" ref="B14"/>
-    <hyperlink r:id="rId10" ref="B15"/>
-    <hyperlink r:id="rId11" ref="B16"/>
-    <hyperlink r:id="rId12" ref="B17"/>
-    <hyperlink r:id="rId13" ref="B18"/>
-    <hyperlink r:id="rId14" ref="B19"/>
-    <hyperlink r:id="rId15" ref="B20"/>
-    <hyperlink r:id="rId16" ref="B21"/>
-    <hyperlink r:id="rId17" ref="B22"/>
-    <hyperlink r:id="rId18" ref="B23"/>
-    <hyperlink r:id="rId19" ref="B24"/>
-    <hyperlink r:id="rId20" ref="B25"/>
-    <hyperlink r:id="rId21" ref="B26"/>
-    <hyperlink r:id="rId22" ref="B27"/>
-    <hyperlink r:id="rId23" ref="B28"/>
-    <hyperlink r:id="rId24" ref="B29"/>
-    <hyperlink r:id="rId25" ref="B30"/>
-    <hyperlink r:id="rId26" ref="B31"/>
-    <hyperlink r:id="rId27" ref="B32"/>
-    <hyperlink r:id="rId28" ref="B33"/>
-    <hyperlink r:id="rId29" ref="B34"/>
-    <hyperlink r:id="rId30" ref="B35"/>
-    <hyperlink r:id="rId31" ref="B36"/>
-    <hyperlink r:id="rId32" ref="B37"/>
-    <hyperlink r:id="rId33" ref="B38"/>
-    <hyperlink r:id="rId34" ref="B39"/>
-    <hyperlink r:id="rId35" ref="B40"/>
-    <hyperlink r:id="rId36" ref="B46"/>
-    <hyperlink r:id="rId37" ref="B47"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B17" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B18" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B19" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B20" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B25" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B26" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B27" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B28" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B29" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B30" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B32" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B33" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B34" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B35" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B36" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B37" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B38" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B39" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B40" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B46" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B47" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
   </hyperlinks>
-  <drawing r:id="rId38"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>